<commit_message>
Making plot for CP04 with consideration to  sqm price
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="760" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B96EFE0-B526-4CEF-A96F-D1D8C2DC0CEA}"/>
+  <xr:revisionPtr revIDLastSave="775" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFC3508-116E-449F-8791-1415BE26C6E3}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>CBi</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>EF/(Ave.m2-price)</t>
+  </si>
+  <si>
+    <t>TJ/m2</t>
   </si>
 </sst>
 </file>
@@ -2752,16 +2755,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2791,16 +2794,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1590675</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4709,8 +4712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E399493D-73F9-461D-8193-76CA6EEF05E5}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C32" sqref="C31:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5179,6 +5182,54 @@
       <c r="J32" s="50">
         <f>E5/E32</f>
         <v>3.0563720511669241</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10">
+      <c r="G34" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10">
+      <c r="G35" s="28">
+        <v>2012</v>
+      </c>
+      <c r="H35">
+        <f>$B$5*C31*10^-6</f>
+        <v>22.298008961008318</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:J35" si="0">$B$5*D31*10^-6</f>
+        <v>12.572458926762478</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>8.9633303389536909</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10">
+      <c r="G36" s="29">
+        <v>2022</v>
+      </c>
+      <c r="H36">
+        <f>$B$5*C32*10^-6</f>
+        <v>30.60044306746212</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36" si="1">$B$5*D32*10^-6</f>
+        <v>15.096717842337531</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36" si="2">$B$5*E32*10^-6</f>
+        <v>9.4807136868180617</v>
       </c>
     </row>
     <row r="51" spans="1:11">

</xml_diff>

<commit_message>
Testing house rent uncertainty stuff
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="775" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFC3508-116E-449F-8791-1415BE26C6E3}"/>
+  <xr:revisionPtr revIDLastSave="1025" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13E86814-753D-491D-A256-3DBBC7DA8F53}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Expenditure" sheetId="2" r:id="rId2"/>
     <sheet name="Housing" sheetId="3" r:id="rId3"/>
+    <sheet name="Housing 2.0" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
   <si>
     <t>CBi</t>
   </si>
@@ -214,17 +215,96 @@
   <si>
     <t>TJ/m2</t>
   </si>
+  <si>
+    <t>Average annual rents per sqm</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>Urban settlements with more than 20,000 inhabitants</t>
+  </si>
+  <si>
+    <t>Urban settlements with between 2,000-19,999 inhabitants</t>
+  </si>
+  <si>
+    <t>Urban settlements with between 200 and 1,999 inhabitants and sparsely populated areas</t>
+  </si>
+  <si>
+    <t>1 room</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>2 rooms</t>
+  </si>
+  <si>
+    <t>3 rooms</t>
+  </si>
+  <si>
+    <t>4 rooms</t>
+  </si>
+  <si>
+    <t>5 rooms or more</t>
+  </si>
+  <si>
+    <t>Average monthly rents</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
+    <t>09895: Rental market survey. Average monthly rents and annual rents per sqm, by price zone and number of rooms (NOK) 2012 - 2023</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>https://www.ssb.no/en/statbank/table/09895</t>
+  </si>
+  <si>
+    <t>Average annual rents per sqm - 2015  [NOK/m2/year]</t>
+  </si>
+  <si>
+    <t>Average monthly rents - 2015 [NOK/month]</t>
+  </si>
+  <si>
+    <t>Energy footprint for CP04</t>
+  </si>
+  <si>
+    <t>EF [Mwh]</t>
+  </si>
+  <si>
+    <t>Sqm [Euro/m2]</t>
+  </si>
+  <si>
+    <t>Average annual rents</t>
+  </si>
+  <si>
+    <t>R [Euro]</t>
+  </si>
+  <si>
+    <t>EF / R</t>
+  </si>
+  <si>
+    <t>EF * Sqm / R</t>
+  </si>
+  <si>
+    <t>CBi * Sqm / R</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +368,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +439,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -459,12 +590,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -517,6 +681,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,17 +748,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1480,6 +1673,1289 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>'2015'</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Housing!G43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Housing!$H$42:$J$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Towns and suburbs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rural areas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Housing!$H$43:$J$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>53.322412684451393</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.215543834743137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.610696892216438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{279D77A1-6499-445F-B0DA-EDEFE6F27CFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="33"/>
+        <c:overlap val="-30"/>
+        <c:axId val="112765960"/>
+        <c:axId val="112768008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="112765960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>EF/(Ave.m2-price)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="112768008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112768008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>2015</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="112765960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>'2015'</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Housing!G53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Housing!$H$52:$J$52</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Towns and suburbs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rural areas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Housing!$H$53:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.69915750897445006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71133212966235726</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71395621166472278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{15929642-BE9C-49B9-9F09-9C4386407189}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="33"/>
+        <c:overlap val="-30"/>
+        <c:axId val="1853594119"/>
+        <c:axId val="1853600263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1853594119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>EF/(Ave.m2-price)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853600263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1853600263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>2015</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853594119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Housing 2.0'!C49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Housing 2.0'!$B$50:$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>EF * Sqm / R</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CBi * Sqm / R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Housing 2.0'!$C$50:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>105.6182290932253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.369900643899086</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{8573BEB4-5B33-4163-B7BD-9E8EE8E57331}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Housing 2.0'!D49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Towns and suburbs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Housing 2.0'!$B$50:$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>EF * Sqm / R</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CBi * Sqm / R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Housing 2.0'!$D$50:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>91.736770268873499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.412567701089259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{92F6F1AB-C068-4251-B8AB-4C5F63997180}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Housing 2.0'!E49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rural areas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Housing 2.0'!$B$50:$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>EF * Sqm / R</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CBi * Sqm / R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Housing 2.0'!$E$50:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>73.300634828246672</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.876110069965051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{55773D7B-07D0-40CC-B600-DAE92BA1AEF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="160"/>
+        <c:overlap val="-30"/>
+        <c:axId val="508577287"/>
+        <c:axId val="508579335"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="508577287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Field1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508579335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="508579335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508577287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1560,6 +3036,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2064,6 +3660,1515 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2900,6 +6005,125 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5" descr="Chart type: Clustered Column. '2015'&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B4428DA-4C0D-FDE8-468F-8E44C8602019}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AA4EBBC2-4E58-9658-7951-3BA3137BD498}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7" descr="Chart type: Clustered Column. '2015'&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C129610C-305D-CB58-AD87-ABE7364C3D19}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{1B4428DA-4C0D-FDE8-468F-8E44C8602019}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2" descr="Chart type: Clustered Column. 'Cities', 'Towns and suburbs', 'Rural areas' by 'Field1'&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C67EA28-9A37-D096-ECED-DB0C0CF15B04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3248,27 +6472,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" s="2" customFormat="1">
-      <c r="B2" s="34">
+      <c r="B2" s="65">
         <v>1</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="H2" s="34">
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="H2" s="65">
         <v>2</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="N2" s="34">
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="N2" s="65">
         <v>3</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
     </row>
     <row r="3" spans="2:18" s="2" customFormat="1">
       <c r="C3" s="2" t="s">
@@ -4710,9 +7934,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E399493D-73F9-461D-8193-76CA6EEF05E5}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -4721,8 +7945,8 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4952,14 +8176,14 @@
       <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="66">
         <v>2012</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="36">
+      <c r="C15" s="68"/>
+      <c r="D15" s="67">
         <v>2022</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="68"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -4979,7 +8203,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="74" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="20" t="s">
@@ -4996,7 +8220,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="43"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="20" t="s">
         <v>45</v>
       </c>
@@ -5011,7 +8235,7 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="43"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="11" t="s">
         <v>47</v>
       </c>
@@ -5026,11 +8250,11 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="16" t="s">
         <v>50</v>
       </c>
@@ -5039,11 +8263,11 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="17" t="s">
         <v>52</v>
       </c>
@@ -5052,11 +8276,11 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="14">
@@ -5124,30 +8348,30 @@
       <c r="B31" s="28">
         <v>2012</v>
       </c>
-      <c r="C31" s="51">
+      <c r="C31" s="38">
         <f>C16*B24</f>
         <v>4472.5324000000001</v>
       </c>
-      <c r="D31" s="51">
+      <c r="D31" s="38">
         <f>AVERAGE(C17:C18)*B24</f>
         <v>2521.7825500000004</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="39">
         <f>C19*B24</f>
         <v>1797.8639000000003</v>
       </c>
       <c r="G31" s="28">
         <v>2012</v>
       </c>
-      <c r="H31" s="48">
+      <c r="H31" s="35">
         <f>C5/C31</f>
         <v>1.8010267007068859</v>
       </c>
-      <c r="I31" s="48">
+      <c r="I31" s="35">
         <f>D5/D31</f>
         <v>2.7725999042866283</v>
       </c>
-      <c r="J31" s="49">
+      <c r="J31" s="36">
         <f>E5/E31</f>
         <v>3.2327926386442818</v>
       </c>
@@ -5156,15 +8380,15 @@
       <c r="B32" s="29">
         <v>2022</v>
       </c>
-      <c r="C32" s="53">
+      <c r="C32" s="40">
         <f>AVERAGE(E16,E17)*B26</f>
         <v>6137.8337999999994</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D32" s="40">
         <f>AVERAGE(E18,E19)*B26</f>
         <v>3028.0981499999998</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="41">
         <f>AVERAGE(E20,E21)*B26</f>
         <v>1901.6405999999999</v>
       </c>
@@ -5179,149 +8403,413 @@
         <f>D5/D32</f>
         <v>2.3090050950830938</v>
       </c>
-      <c r="J32" s="50">
+      <c r="J32" s="37">
         <f>E5/E32</f>
         <v>3.0563720511669241</v>
       </c>
     </row>
-    <row r="34" spans="7:10">
+    <row r="34" spans="2:10">
       <c r="G34" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I34" s="25" t="s">
+      <c r="I34" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="47" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="7:10">
-      <c r="G35" s="28">
+    <row r="35" spans="2:10">
+      <c r="G35" s="14">
         <v>2012</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="52">
         <f>$B$5*C31*10^-6</f>
         <v>22.298008961008318</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="46">
         <f t="shared" ref="I35:J35" si="0">$B$5*D31*10^-6</f>
         <v>12.572458926762478</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="47">
         <f t="shared" si="0"/>
         <v>8.9633303389536909</v>
       </c>
     </row>
-    <row r="36" spans="7:10">
-      <c r="G36" s="29">
+    <row r="36" spans="2:10">
+      <c r="G36" s="15">
         <v>2022</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="15">
         <f>$B$5*C32*10^-6</f>
         <v>30.60044306746212</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="53">
         <f t="shared" ref="I36" si="1">$B$5*D32*10^-6</f>
         <v>15.096717842337531</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="54">
         <f t="shared" ref="J36" si="2">$B$5*E32*10^-6</f>
         <v>9.4807136868180617</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="44"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="46"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="45"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="46"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="45"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="45"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="45"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
+    <row r="39" spans="2:10">
+      <c r="C39" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="C40" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="72" customHeight="1">
+      <c r="C41" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J42" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="43">
+        <v>1550</v>
+      </c>
+      <c r="D43" s="43">
+        <v>1390</v>
+      </c>
+      <c r="E43" s="43">
+        <v>1170</v>
+      </c>
+      <c r="G43" s="51">
+        <v>2015</v>
+      </c>
+      <c r="H43" s="50">
+        <f>C5/(AVERAGE(C43:C46)*$B$25)</f>
+        <v>53.322412684451393</v>
+      </c>
+      <c r="I43" s="48">
+        <f t="shared" ref="I43:J43" si="3">D5/(AVERAGE(D43:D46)*$B$25)</f>
+        <v>54.215543834743137</v>
+      </c>
+      <c r="J43" s="49">
+        <f t="shared" si="3"/>
+        <v>56.610696892216438</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="43">
+        <v>1430</v>
+      </c>
+      <c r="D44" s="43">
+        <v>1200</v>
+      </c>
+      <c r="E44" s="43">
+        <v>990</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="43">
+        <v>1250</v>
+      </c>
+      <c r="D45" s="43">
+        <v>1120</v>
+      </c>
+      <c r="E45" s="43">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="43">
+        <v>1170</v>
+      </c>
+      <c r="D46" s="43">
+        <v>900</v>
+      </c>
+      <c r="E46" s="43">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="B49" s="55"/>
+      <c r="C49" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="B50" s="55"/>
+      <c r="C50" s="42">
+        <v>2015</v>
+      </c>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+    </row>
+    <row r="51" spans="1:10" ht="74.25" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="34"/>
+      <c r="B52" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="55">
+        <v>5760</v>
+      </c>
+      <c r="D52" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="34"/>
+      <c r="G52" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H52" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J52" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="34"/>
+      <c r="B53" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="55">
+        <v>6550</v>
+      </c>
+      <c r="D53" s="55">
+        <v>5990</v>
+      </c>
+      <c r="E53" s="55">
+        <v>5400</v>
+      </c>
+      <c r="F53" s="34"/>
+      <c r="G53" s="51">
+        <v>2015</v>
+      </c>
+      <c r="H53" s="50">
+        <f>C5/(AVERAGE(C53:C56)*12*$B$25)</f>
+        <v>0.69915750897445006</v>
+      </c>
+      <c r="I53" s="50">
+        <f t="shared" ref="I53:J53" si="4">D5/(AVERAGE(D53:D56)*12*$B$25)</f>
+        <v>0.71133212966235726</v>
+      </c>
+      <c r="J53" s="50">
+        <f t="shared" si="4"/>
+        <v>0.71395621166472278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="34"/>
+      <c r="B54" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="55">
+        <v>8250</v>
+      </c>
+      <c r="D54" s="55">
+        <v>7090</v>
+      </c>
+      <c r="E54" s="55">
+        <v>5870</v>
+      </c>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="B55" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="55">
+        <v>8760</v>
+      </c>
+      <c r="D55" s="55">
+        <v>7860</v>
+      </c>
+      <c r="E55" s="55">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="B56" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="55">
+        <v>10760</v>
+      </c>
+      <c r="D56" s="55">
+        <v>8340</v>
+      </c>
+      <c r="E56" s="55">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60" s="55"/>
+      <c r="C60" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="55"/>
+      <c r="C61" s="42">
+        <v>2015</v>
+      </c>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55"/>
+    </row>
+    <row r="62" spans="1:10" ht="76.5">
+      <c r="B62" s="55"/>
+      <c r="C62" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="B63" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="55">
+        <v>5760</v>
+      </c>
+      <c r="D63" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="B64" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="55">
+        <v>6550</v>
+      </c>
+      <c r="D64" s="55">
+        <v>5990</v>
+      </c>
+      <c r="E64" s="55">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="55">
+        <v>8250</v>
+      </c>
+      <c r="D65" s="55">
+        <v>7090</v>
+      </c>
+      <c r="E65" s="55">
+        <v>5870</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="55">
+        <v>8760</v>
+      </c>
+      <c r="D66" s="55">
+        <v>7860</v>
+      </c>
+      <c r="E66" s="55">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="55">
+        <v>10760</v>
+      </c>
+      <c r="D67" s="55">
+        <v>8340</v>
+      </c>
+      <c r="E67" s="55">
+        <v>6780</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5341,4 +8829,664 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7463AF02-F5DD-486C-9004-F4B4453F225B}">
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" ht="88.5" customHeight="1">
+      <c r="A5" s="75"/>
+      <c r="B5" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="75"/>
+      <c r="B6" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="75"/>
+      <c r="B7" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="43">
+        <v>1550</v>
+      </c>
+      <c r="D7" s="43">
+        <v>1390</v>
+      </c>
+      <c r="E7" s="43">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="75"/>
+      <c r="B8" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="43">
+        <v>1430</v>
+      </c>
+      <c r="D8" s="43">
+        <v>1200</v>
+      </c>
+      <c r="E8" s="43">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="75"/>
+      <c r="B9" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="43">
+        <v>1250</v>
+      </c>
+      <c r="D9" s="43">
+        <v>1120</v>
+      </c>
+      <c r="E9" s="43">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="75"/>
+      <c r="B10" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="43">
+        <v>1170</v>
+      </c>
+      <c r="D10" s="43">
+        <v>900</v>
+      </c>
+      <c r="E10" s="43">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="55"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+    </row>
+    <row r="13" spans="1:5" ht="90" customHeight="1">
+      <c r="B13" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="55">
+        <v>5760</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="55">
+        <v>6550</v>
+      </c>
+      <c r="D15" s="55">
+        <v>5990</v>
+      </c>
+      <c r="E15" s="55">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="55">
+        <v>8250</v>
+      </c>
+      <c r="D16" s="55">
+        <v>7090</v>
+      </c>
+      <c r="E16" s="55">
+        <v>5870</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="55">
+        <v>8760</v>
+      </c>
+      <c r="D17" s="55">
+        <v>7860</v>
+      </c>
+      <c r="E17" s="55">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="B18" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="55">
+        <v>10760</v>
+      </c>
+      <c r="D18" s="55">
+        <v>8340</v>
+      </c>
+      <c r="E18" s="55">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="B19" s="42"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="67"/>
+      <c r="D21" s="68"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C22">
+        <v>0.13370000000000001</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C23" s="58">
+        <v>0.1119</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24" s="15">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="53">
+        <v>9.3299999999999994E-2</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="19">
+        <v>879.45386608450497</v>
+      </c>
+      <c r="C28" s="19">
+        <v>433.50550050279702</v>
+      </c>
+      <c r="D28" s="19">
+        <v>470.99775721815098</v>
+      </c>
+      <c r="E28" s="19">
+        <v>506.87141817981399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="19">
+        <v>46.5641180203896</v>
+      </c>
+      <c r="C29" s="19">
+        <v>5.7381637816237401</v>
+      </c>
+      <c r="D29" s="19">
+        <v>5.4947570979793996</v>
+      </c>
+      <c r="E29" s="19">
+        <v>5.8960368368764202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="19">
+        <v>35.137031853302503</v>
+      </c>
+      <c r="C30" s="19">
+        <v>9.3014543803985994</v>
+      </c>
+      <c r="D30" s="19">
+        <v>8.7710488794204498</v>
+      </c>
+      <c r="E30" s="19">
+        <v>6.9038030768585497</v>
+      </c>
+      <c r="G30">
+        <v>16000</v>
+      </c>
+      <c r="I30">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="64">
+        <v>4985.5444224413704</v>
+      </c>
+      <c r="C31" s="10">
+        <v>8055.1502721766501</v>
+      </c>
+      <c r="D31" s="10">
+        <v>6991.8940567616901</v>
+      </c>
+      <c r="E31" s="10">
+        <v>5812.1211812043002</v>
+      </c>
+      <c r="G31">
+        <v>45</v>
+      </c>
+      <c r="H31">
+        <v>38</v>
+      </c>
+      <c r="I31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="19">
+        <v>603.95394256237705</v>
+      </c>
+      <c r="C32" s="19">
+        <v>132.31310235587199</v>
+      </c>
+      <c r="D32" s="19">
+        <v>158.98479222122401</v>
+      </c>
+      <c r="E32" s="19">
+        <v>158.22163937470199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="19">
+        <v>105.841415679102</v>
+      </c>
+      <c r="C33" s="19">
+        <v>12.076843633507901</v>
+      </c>
+      <c r="D33" s="19">
+        <v>12.970095495174901</v>
+      </c>
+      <c r="E33" s="19">
+        <v>11.553310831008501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="19">
+        <v>1220.2202521422601</v>
+      </c>
+      <c r="C34" s="19">
+        <v>891.07858364952199</v>
+      </c>
+      <c r="D34" s="19">
+        <v>1013.47511140663</v>
+      </c>
+      <c r="E34" s="19">
+        <v>1284.0031238531401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="19">
+        <v>90.817753347897593</v>
+      </c>
+      <c r="C35" s="19">
+        <v>7.0465651230986701</v>
+      </c>
+      <c r="D35" s="19">
+        <v>7.8315572036650201</v>
+      </c>
+      <c r="E35" s="19">
+        <v>8.7237707420061898</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="19">
+        <v>1146.6233518224501</v>
+      </c>
+      <c r="C36" s="19">
+        <v>497.16687161664601</v>
+      </c>
+      <c r="D36" s="19">
+        <v>541.22505216368802</v>
+      </c>
+      <c r="E36" s="19">
+        <v>455.58874182764902</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="19">
+        <v>133.28489008696499</v>
+      </c>
+      <c r="C37" s="19">
+        <v>1.8249878076119199</v>
+      </c>
+      <c r="D37" s="19">
+        <v>1.2098587875986799</v>
+      </c>
+      <c r="E37" s="19">
+        <v>0.58195811322865798</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="19">
+        <v>19.988445783937198</v>
+      </c>
+      <c r="C38" s="19">
+        <v>4.0141121080311999</v>
+      </c>
+      <c r="D38" s="19">
+        <v>3.1751982044720299</v>
+      </c>
+      <c r="E38" s="19">
+        <v>2.4436998765703901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="19">
+        <v>3835.8189366430202</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1050.4300655555001</v>
+      </c>
+      <c r="D39" s="19">
+        <v>1114.1966343178301</v>
+      </c>
+      <c r="E39" s="19">
+        <v>988.14555067976596</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="C42" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="1">
+        <f>C31</f>
+        <v>8055.1502721766501</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" ref="D43:E43" si="0">D31</f>
+        <v>6991.8940567616901</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>5812.1211812043002</v>
+      </c>
+      <c r="G43" s="1">
+        <f>B31</f>
+        <v>4985.5444224413704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="1">
+        <f>AVERAGE(C7:C10)*$C$23</f>
+        <v>151.065</v>
+      </c>
+      <c r="D44" s="1">
+        <f>AVERAGE(D7:D10)*$C$23</f>
+        <v>128.96475000000001</v>
+      </c>
+      <c r="E44" s="1">
+        <f>AVERAGE(E7:E10)*$C$23</f>
+        <v>102.66825</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45">
+        <f>AVERAGE(C15:C18)*12*$C$23</f>
+        <v>11521.224</v>
+      </c>
+      <c r="D45">
+        <f>AVERAGE(D15:D18)*12*$C$23</f>
+        <v>9829.2960000000003</v>
+      </c>
+      <c r="E45">
+        <f>AVERAGE(E15:E18)*12*$C$23</f>
+        <v>8140.7250000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="63"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48">
+        <f>C43/C45</f>
+        <v>0.69915750897445006</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:E48" si="1">D43/D45</f>
+        <v>0.71133212966235726</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0.71395621166472278</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="C49" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50">
+        <f>C43*C44/C45</f>
+        <v>105.6182290932253</v>
+      </c>
+      <c r="D50">
+        <f>D43*D44/D45</f>
+        <v>91.736770268873499</v>
+      </c>
+      <c r="E50">
+        <f>E43*E44/E45</f>
+        <v>73.300634828246672</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51">
+        <f>$B$31*C44/C45</f>
+        <v>65.369900643899086</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:E51" si="2">$B$31*D44/D45</f>
+        <v>65.412567701089259</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>62.876110069965051</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A5:A10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F199651D-BCD5-46BC-B4E3-E97DC314FB91}"/>
+    <hyperlink ref="D23" r:id="rId2" xr:uid="{F171048F-2836-4036-ACA5-E6CEAC312A13}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{3AE6767E-119F-47EF-B493-5AF51D9A3C8B}"/>
+    <hyperlink ref="D24" r:id="rId4" xr:uid="{EB50B43C-FDBF-49F3-A977-9825CF0E04E1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>